<commit_message>
* Ajustes de estilos * Actualización de socios para que tengan los nombres * Descarga de imágenes de socios * Inclusión de videos de fanvida empresarial y rural * Otros ajustes generales
</commit_message>
<xml_diff>
--- a/assets/consejos.xlsx
+++ b/assets/consejos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Personal)\Proyectos\FanCampo\dev\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F43FEEAB-8AC1-4F0D-AD19-354FC6BAEF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DBFFF9-90C8-411B-826F-1669DB8B5125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40080" yWindow="-8250" windowWidth="16440" windowHeight="29040" xr2:uid="{63C9C974-292F-4EBA-9C08-E5656FFA8A86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{63C9C974-292F-4EBA-9C08-E5656FFA8A86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1642,7 +1638,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>Sr. Helios Serrato Pérez</a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -1666,10 +1662,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>Propietario</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1200"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -1682,7 +1675,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>Ing. Noel Javier Ramírez Mejía</a:t>
+            <a:t>Suplente</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -1706,10 +1699,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>Suplente</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1200"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -1798,7 +1788,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Sr. José Ernestino Mazariegos Zenteno</a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -1816,16 +1806,59 @@
     </dgm:pt>
     <dgm:pt modelId="{05D04BB6-2C15-444A-9CD5-517594D01B72}" type="sibTrans" cxnId="{7E9B00FC-BB57-4060-9FDA-DAE319564E52}">
       <dgm:prSet custT="1"/>
-      <dgm:spPr/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:sysClr>
+        </a:solidFill>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="4EA72E">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:srgbClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dgm:spPr>
       <dgm:t>
-        <a:bodyPr/>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Propietario</a:t>
-          </a:r>
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX" sz="500" kern="1200">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -1838,7 +1871,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>Ing. Omar Martín Arjona Ceballos</a:t>
+            <a:t>Suplente</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -1862,10 +1895,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>Suplente</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1200"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -1914,7 +1944,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Ing. Homero de Jesús de la Llata García</a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -1938,10 +1968,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Propietario</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -1954,7 +1981,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>MVZ. Jorge Alejandro Ugalde Tinoco</a:t>
+            <a:t>Suplente</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -1972,16 +1999,59 @@
     </dgm:pt>
     <dgm:pt modelId="{A2485CFF-52AC-44DF-8BEF-B4FF100690D6}" type="sibTrans" cxnId="{95B7157B-B765-4080-84AD-B16626E223B5}">
       <dgm:prSet custT="1"/>
-      <dgm:spPr/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:sysClr>
+        </a:solidFill>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="4EA72E">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:srgbClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dgm:spPr>
       <dgm:t>
-        <a:bodyPr/>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Suplente</a:t>
-          </a:r>
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX" sz="500" kern="1200">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -2107,7 +2177,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{BA5351DA-6F80-47C8-BBCF-ADA0411DC43C}" type="pres">
-      <dgm:prSet presAssocID="{B5B041B2-0BA1-4550-89AB-52A5676E007E}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="0" presStyleCnt="6">
+      <dgm:prSet presAssocID="{B5B041B2-0BA1-4550-89AB-52A5676E007E}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="0" presStyleCnt="6" custFlipVert="1" custScaleY="28169" custLinFactNeighborX="-15521" custLinFactNeighborY="-56658">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -2152,13 +2222,21 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{1DD63F7F-9D5F-401A-963D-31060E539491}" type="pres">
-      <dgm:prSet presAssocID="{903332FD-8219-42C1-A486-8FD7ACAEBEBB}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="1" presStyleCnt="6">
+      <dgm:prSet presAssocID="{903332FD-8219-42C1-A486-8FD7ACAEBEBB}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="1" presStyleCnt="6" custScaleY="31188" custLinFactNeighborX="-17074" custLinFactNeighborY="-62054">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
-      <dgm:spPr/>
+      <dgm:spPr>
+        <a:xfrm>
+          <a:off x="1873108" y="2657582"/>
+          <a:ext cx="1150645" cy="68816"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </dgm:spPr>
     </dgm:pt>
     <dgm:pt modelId="{8C98DAE3-10EE-44E7-B392-736C745D59CF}" type="pres">
       <dgm:prSet presAssocID="{903332FD-8219-42C1-A486-8FD7ACAEBEBB}" presName="rootConnector3" presStyleLbl="asst2" presStyleIdx="0" presStyleCnt="0"/>
@@ -2243,13 +2321,21 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{88CFCF9E-3D38-4F8A-BED2-E36F336DF41F}" type="pres">
-      <dgm:prSet presAssocID="{29CDD68F-F1B6-4B80-AB88-8DBA2D6A130E}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="2" presStyleCnt="6">
+      <dgm:prSet presAssocID="{29CDD68F-F1B6-4B80-AB88-8DBA2D6A130E}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="2" presStyleCnt="6" custScaleY="29127" custLinFactNeighborX="-16556" custLinFactNeighborY="-62054">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
-      <dgm:spPr/>
+      <dgm:spPr>
+        <a:xfrm>
+          <a:off x="3594322" y="2669130"/>
+          <a:ext cx="1150645" cy="45720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </dgm:spPr>
     </dgm:pt>
     <dgm:pt modelId="{E979C001-E09A-4369-993C-BD25F4E62730}" type="pres">
       <dgm:prSet presAssocID="{29CDD68F-F1B6-4B80-AB88-8DBA2D6A130E}" presName="rootConnector3" presStyleLbl="asst2" presStyleIdx="0" presStyleCnt="0"/>
@@ -2288,7 +2374,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{FFF0DEBF-825F-46FE-B32D-91D5510B0FF6}" type="pres">
-      <dgm:prSet presAssocID="{C7B50723-0F7F-4384-A839-B9AE0EC52079}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="3" presStyleCnt="6">
+      <dgm:prSet presAssocID="{C7B50723-0F7F-4384-A839-B9AE0EC52079}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="3" presStyleCnt="6" custScaleY="31186" custLinFactNeighborX="-16039" custLinFactNeighborY="-64752">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -2379,7 +2465,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{8177B874-6A91-4226-9047-656094C7FCA8}" type="pres">
-      <dgm:prSet presAssocID="{1E8CE79C-90A2-4936-9DD3-8FE55ED0FD1B}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="4" presStyleCnt="6">
+      <dgm:prSet presAssocID="{1E8CE79C-90A2-4936-9DD3-8FE55ED0FD1B}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="4" presStyleCnt="6" custScaleY="31187" custLinFactNeighborX="-17590" custLinFactNeighborY="-67450">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -2424,7 +2510,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{2A16CEDE-4BA4-49BA-AE16-DDE0D3D966CA}" type="pres">
-      <dgm:prSet presAssocID="{3C88D9C2-1369-4887-BECA-3594AA7999D6}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="5" presStyleCnt="6">
+      <dgm:prSet presAssocID="{3C88D9C2-1369-4887-BECA-3594AA7999D6}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="5" presStyleCnt="6" custScaleY="28126" custLinFactNeighborX="-15521" custLinFactNeighborY="-62054">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -2649,7 +2735,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>Ing. Lauro Aniceto Flores Ramos</a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -2673,10 +2759,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>Propietario</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1200"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -2689,7 +2772,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>MVZ. Rene Loyo García</a:t>
+            <a:t>Suplente</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -2713,10 +2796,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>Suplente</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1200"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -2805,7 +2885,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>MVZ. Tito Germán de Coss Tovilla</a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -2829,10 +2909,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Propietario</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -2845,7 +2922,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>Ing. Jorge Antonio Salazar Barragán</a:t>
+            <a:t>Suplente</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -2869,10 +2946,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200"/>
-            <a:t>Suplente</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1200"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -2921,7 +2995,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Lic. Gustavo Rodríguez Cabrales</a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -2945,10 +3019,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Propietario</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -2961,7 +3032,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>LAE. Esteban Abraham Macari</a:t>
+            <a:t>Suplente</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -2985,10 +3056,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Suplente</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
@@ -3114,7 +3182,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{BA5351DA-6F80-47C8-BBCF-ADA0411DC43C}" type="pres">
-      <dgm:prSet presAssocID="{B5B041B2-0BA1-4550-89AB-52A5676E007E}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="0" presStyleCnt="6">
+      <dgm:prSet presAssocID="{B5B041B2-0BA1-4550-89AB-52A5676E007E}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="0" presStyleCnt="6" custScaleY="26290" custLinFactNeighborX="-17826" custLinFactNeighborY="-52058">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3159,7 +3227,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{1DD63F7F-9D5F-401A-963D-31060E539491}" type="pres">
-      <dgm:prSet presAssocID="{903332FD-8219-42C1-A486-8FD7ACAEBEBB}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="1" presStyleCnt="6">
+      <dgm:prSet presAssocID="{903332FD-8219-42C1-A486-8FD7ACAEBEBB}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="1" presStyleCnt="6" custScaleY="26289" custLinFactNeighborX="-16400" custLinFactNeighborY="-55776">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3250,7 +3318,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{88CFCF9E-3D38-4F8A-BED2-E36F336DF41F}" type="pres">
-      <dgm:prSet presAssocID="{29CDD68F-F1B6-4B80-AB88-8DBA2D6A130E}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="2" presStyleCnt="6">
+      <dgm:prSet presAssocID="{29CDD68F-F1B6-4B80-AB88-8DBA2D6A130E}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="2" presStyleCnt="6" custFlipVert="1" custScaleY="26287" custLinFactNeighborX="-16400" custLinFactNeighborY="-48339">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3295,7 +3363,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{FFF0DEBF-825F-46FE-B32D-91D5510B0FF6}" type="pres">
-      <dgm:prSet presAssocID="{C7B50723-0F7F-4384-A839-B9AE0EC52079}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="3" presStyleCnt="6">
+      <dgm:prSet presAssocID="{C7B50723-0F7F-4384-A839-B9AE0EC52079}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="3" presStyleCnt="6" custScaleY="26288" custLinFactNeighborX="-14974" custLinFactNeighborY="-52057">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3386,7 +3454,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{8177B874-6A91-4226-9047-656094C7FCA8}" type="pres">
-      <dgm:prSet presAssocID="{1E8CE79C-90A2-4936-9DD3-8FE55ED0FD1B}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="4" presStyleCnt="6">
+      <dgm:prSet presAssocID="{1E8CE79C-90A2-4936-9DD3-8FE55ED0FD1B}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="4" presStyleCnt="6" custScaleY="26288" custLinFactNeighborX="-16400" custLinFactNeighborY="-55776">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3431,7 +3499,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{2A16CEDE-4BA4-49BA-AE16-DDE0D3D966CA}" type="pres">
-      <dgm:prSet presAssocID="{3C88D9C2-1369-4887-BECA-3594AA7999D6}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="5" presStyleCnt="6">
+      <dgm:prSet presAssocID="{3C88D9C2-1369-4887-BECA-3594AA7999D6}" presName="titleText3" presStyleLbl="fgAcc2" presStyleIdx="5" presStyleCnt="6" custScaleY="26290" custLinFactNeighborX="-15687" custLinFactNeighborY="-52058">
         <dgm:presLayoutVars>
           <dgm:chMax val="0"/>
           <dgm:chPref val="0"/>
@@ -3612,8 +3680,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8426832" y="1856894"/>
-          <a:ext cx="217612" cy="637637"/>
+          <a:off x="8536919" y="1898327"/>
+          <a:ext cx="220455" cy="645967"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3627,10 +3695,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="637637"/>
+                <a:pt x="0" y="645967"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="217612" y="637637"/>
+                <a:pt x="220455" y="645967"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3671,8 +3739,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8209219" y="1856894"/>
-          <a:ext cx="217612" cy="637637"/>
+          <a:off x="8316463" y="1898327"/>
+          <a:ext cx="220455" cy="645967"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3683,13 +3751,13 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="217612" y="0"/>
+                <a:pt x="220455" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="217612" y="637637"/>
+                <a:pt x="220455" y="645967"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="637637"/>
+                <a:pt x="0" y="645967"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3730,8 +3798,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5008363" y="816152"/>
-          <a:ext cx="3418469" cy="381116"/>
+          <a:off x="5073791" y="843989"/>
+          <a:ext cx="3463127" cy="386095"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3745,13 +3813,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="227204"/>
+                <a:pt x="0" y="230172"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="3418469" y="227204"/>
+                <a:pt x="3463127" y="230172"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="3418469" y="381116"/>
+                <a:pt x="3463127" y="386095"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3792,8 +3860,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5002936" y="1856894"/>
-          <a:ext cx="223039" cy="637637"/>
+          <a:off x="5068294" y="1898327"/>
+          <a:ext cx="225953" cy="645967"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3807,10 +3875,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="637637"/>
+                <a:pt x="0" y="645967"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="223039" y="637637"/>
+                <a:pt x="225953" y="645967"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3851,8 +3919,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4790750" y="1856894"/>
-          <a:ext cx="212186" cy="637637"/>
+          <a:off x="4853336" y="1898327"/>
+          <a:ext cx="214958" cy="645967"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3863,13 +3931,13 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="212186" y="0"/>
+                <a:pt x="214958" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="212186" y="637637"/>
+                <a:pt x="214958" y="645967"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="637637"/>
+                <a:pt x="0" y="645967"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3910,8 +3978,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4957216" y="816152"/>
-          <a:ext cx="91440" cy="381116"/>
+          <a:off x="5022574" y="843989"/>
+          <a:ext cx="91440" cy="386095"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3922,16 +3990,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="51146" y="0"/>
+                <a:pt x="51217" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="51146" y="227204"/>
+                <a:pt x="51217" y="230172"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="45720" y="227204"/>
+                <a:pt x="45720" y="230172"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="45720" y="381116"/>
+                <a:pt x="45720" y="386095"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3972,8 +4040,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1589893" y="1856894"/>
-          <a:ext cx="217612" cy="637637"/>
+          <a:off x="1610664" y="1898327"/>
+          <a:ext cx="220455" cy="645967"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3987,10 +4055,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="637637"/>
+                <a:pt x="0" y="645967"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="217612" y="637637"/>
+                <a:pt x="220455" y="645967"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4031,8 +4099,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1372280" y="1856894"/>
-          <a:ext cx="217612" cy="637637"/>
+          <a:off x="1390208" y="1898327"/>
+          <a:ext cx="220455" cy="645967"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4043,13 +4111,13 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="217612" y="0"/>
+                <a:pt x="220455" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="217612" y="637637"/>
+                <a:pt x="220455" y="645967"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="637637"/>
+                <a:pt x="0" y="645967"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4090,8 +4158,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1589893" y="816152"/>
-          <a:ext cx="3418469" cy="381116"/>
+          <a:off x="1610664" y="843989"/>
+          <a:ext cx="3463127" cy="386095"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4102,16 +4170,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="3418469" y="0"/>
+                <a:pt x="3463127" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="3418469" y="227204"/>
+                <a:pt x="3463127" y="230172"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="227204"/>
+                <a:pt x="0" y="230172"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="381116"/>
+                <a:pt x="0" y="386095"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4152,8 +4220,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4371358" y="156527"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="4428465" y="175747"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4195,7 +4263,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -4219,8 +4287,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4371358" y="156527"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="4428465" y="175747"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{5F1A3974-34FA-4443-A94B-5F13166B2718}">
@@ -4230,8 +4298,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4626160" y="669569"/>
-          <a:ext cx="1146607" cy="219875"/>
+          <a:off x="4686596" y="695491"/>
+          <a:ext cx="1161586" cy="222747"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4296,8 +4364,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4626160" y="669569"/>
-        <a:ext cx="1146607" cy="219875"/>
+        <a:off x="4686596" y="695491"/>
+        <a:ext cx="1161586" cy="222747"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{9ED8802D-6851-4628-9575-5CD454ED0A4D}">
@@ -4307,8 +4375,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="952889" y="1197269"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="965338" y="1230085"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4350,7 +4418,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -4374,8 +4442,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="952889" y="1197269"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="965338" y="1230085"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F72357A0-A2DF-42C9-9A9D-2F404917D7F8}">
@@ -4385,8 +4453,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1048175" y="1629750"/>
-          <a:ext cx="1146607" cy="56290"/>
+          <a:off x="1061868" y="1668215"/>
+          <a:ext cx="1161586" cy="57025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4448,8 +4516,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1048175" y="1629750"/>
-        <a:ext cx="1146607" cy="56290"/>
+        <a:off x="1061868" y="1668215"/>
+        <a:ext cx="1161586" cy="57025"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{13E60599-934D-435E-972C-34B728BDD199}">
@@ -4459,8 +4527,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="98272" y="2164719"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="99556" y="2210174"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4502,7 +4570,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -4521,13 +4589,13 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Ing. Homero de Jesús de la Llata García</a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="98272" y="2164719"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="99556" y="2210174"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{BA5351DA-6F80-47C8-BBCF-ADA0411DC43C}">
@@ -4536,9 +4604,9 @@
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm>
-          <a:off x="353074" y="2677761"/>
-          <a:ext cx="1146607" cy="219875"/>
+        <a:xfrm flipV="1">
+          <a:off x="177396" y="2683715"/>
+          <a:ext cx="1161586" cy="62745"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4596,15 +4664,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Propietario</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1100" kern="1200"/>
         </a:p>
       </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="353074" y="2677761"/>
-        <a:ext cx="1146607" cy="219875"/>
+      <dsp:txXfrm rot="10800000">
+        <a:off x="177396" y="2683715"/>
+        <a:ext cx="1161586" cy="62745"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{3247D56F-F64A-4433-88EA-A164DC2F9628}">
@@ -4614,8 +4679,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1807506" y="2164719"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="1831120" y="2210174"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4657,7 +4722,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -4676,13 +4741,13 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>MVZ. Jorge Alejandro Ugalde Tinoco</a:t>
+            <a:t>Suplente</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1807506" y="2164719"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="1831120" y="2210174"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{1DD63F7F-9D5F-401A-963D-31060E539491}">
@@ -4692,8 +4757,172 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2062308" y="2677761"/>
-          <a:ext cx="1146607" cy="219875"/>
+          <a:off x="1890921" y="2668333"/>
+          <a:ext cx="1161586" cy="69470"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:sysClr>
+        </a:solidFill>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="4EA72E">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:srgbClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX" sz="500" kern="1200">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="1890921" y="2668333"/>
+        <a:ext cx="1161586" cy="69470"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{5DD61981-23C1-45CB-816C-E7FC3C54CBAE}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4422968" y="1230085"/>
+          <a:ext cx="1290652" cy="668242"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
+            <a:t>Secretario</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4422968" y="1230085"/>
+        <a:ext cx="1290652" cy="668242"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{DAFF9247-F0DB-441E-8679-2A16A7188832}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4475922" y="1658227"/>
+          <a:ext cx="1183575" cy="57025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4734,12 +4963,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="27940" tIns="6985" rIns="27940" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4751,26 +4980,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Suplente</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2062308" y="2677761"/>
-        <a:ext cx="1146607" cy="219875"/>
+      <dsp:txXfrm rot="10800000">
+        <a:off x="4475922" y="1658227"/>
+        <a:ext cx="1183575" cy="57025"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{5DD61981-23C1-45CB-816C-E7FC3C54CBAE}">
+    <dsp:sp modelId="{22BD4AE8-0E96-4AF3-941E-AFBF8514EA1F}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4365932" y="1197269"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="3562683" y="2210174"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4812,7 +5038,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -4831,24 +5057,188 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Secretario</a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4365932" y="1197269"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="3562683" y="2210174"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{DAFF9247-F0DB-441E-8679-2A16A7188832}">
+    <dsp:sp modelId="{88CFCF9E-3D38-4F8A-BED2-E36F336DF41F}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4418203" y="1619890"/>
-          <a:ext cx="1168313" cy="56290"/>
+        <a:xfrm>
+          <a:off x="3628501" y="2670628"/>
+          <a:ext cx="1161586" cy="64879"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:sysClr>
+        </a:solidFill>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="4EA72E">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:srgbClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX" sz="500" kern="1200">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3628501" y="2670628"/>
+        <a:ext cx="1161586" cy="64879"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{99276632-6755-4F04-94C2-7FD5F7A54AE1}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="5294247" y="2210174"/>
+          <a:ext cx="1290652" cy="668242"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
+            <a:t>Suplente</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="5294247" y="2210174"/>
+        <a:ext cx="1290652" cy="668242"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{FFF0DEBF-825F-46FE-B32D-91D5510B0FF6}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="5366071" y="2662325"/>
+          <a:ext cx="1161586" cy="69466"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4889,12 +5279,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="30480" tIns="7620" rIns="30480" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4906,23 +5296,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="es-MX" sz="500" kern="1200"/>
+          <a:endParaRPr lang="es-MX" sz="1200" kern="1200"/>
         </a:p>
       </dsp:txBody>
-      <dsp:txXfrm rot="10800000">
-        <a:off x="4418203" y="1619890"/>
-        <a:ext cx="1168313" cy="56290"/>
+      <dsp:txXfrm>
+        <a:off x="5366071" y="2662325"/>
+        <a:ext cx="1161586" cy="69466"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{22BD4AE8-0E96-4AF3-941E-AFBF8514EA1F}">
+    <dsp:sp modelId="{15ECEB10-3A4A-46CF-BC89-CA90D33E60BE}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3516741" y="2164719"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="7891593" y="1230085"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4964,7 +5354,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -4983,24 +5373,24 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Sr. José Ernestino Mazariegos Zenteno</a:t>
+            <a:t>Tesorero</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3516741" y="2164719"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="7891593" y="1230085"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{88CFCF9E-3D38-4F8A-BED2-E36F336DF41F}">
+    <dsp:sp modelId="{DDC5D6E6-CDD3-4B39-A20A-FECE67469267}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3771543" y="2677761"/>
-          <a:ext cx="1146607" cy="219875"/>
+          <a:off x="7955541" y="1670109"/>
+          <a:ext cx="1161586" cy="57025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5041,12 +5431,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="27940" tIns="6985" rIns="27940" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5058,26 +5448,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Propietario</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3771543" y="2677761"/>
-        <a:ext cx="1146607" cy="219875"/>
+        <a:off x="7955541" y="1670109"/>
+        <a:ext cx="1161586" cy="57025"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{99276632-6755-4F04-94C2-7FD5F7A54AE1}">
+    <dsp:sp modelId="{5DC9F435-2CE6-4405-AD55-3577C8FF29E2}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5225976" y="2164719"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="7025811" y="2210174"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5119,7 +5506,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -5138,24 +5525,24 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>Ing. Omar Martín Arjona Ceballos</a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5225976" y="2164719"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="7025811" y="2210174"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{FFF0DEBF-825F-46FE-B32D-91D5510B0FF6}">
+    <dsp:sp modelId="{8177B874-6A91-4226-9047-656094C7FCA8}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5480777" y="2677761"/>
-          <a:ext cx="1146607" cy="219875"/>
+          <a:off x="7079618" y="2656314"/>
+          <a:ext cx="1161586" cy="69468"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5213,26 +5600,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>Suplente</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1200" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5480777" y="2677761"/>
-        <a:ext cx="1146607" cy="219875"/>
+        <a:off x="7079618" y="2656314"/>
+        <a:ext cx="1161586" cy="69468"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{15ECEB10-3A4A-46CF-BC89-CA90D33E60BE}">
+    <dsp:sp modelId="{37FA40A9-D75C-44AF-B413-F0C3A4F49306}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7789827" y="1197269"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="8757375" y="2210174"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5274,12 +5658,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5292,25 +5676,25 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Tesorero</a:t>
+            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
+            <a:t>Suplente</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7789827" y="1197269"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="8757375" y="2210174"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{DDC5D6E6-CDD3-4B39-A20A-FECE67469267}">
+    <dsp:sp modelId="{2A16CEDE-4BA4-49BA-AE16-DDE0D3D966CA}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7852951" y="1631619"/>
-          <a:ext cx="1146607" cy="56290"/>
+          <a:off x="8835216" y="2671743"/>
+          <a:ext cx="1161586" cy="62649"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5351,12 +5735,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="30480" tIns="7620" rIns="30480" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5368,23 +5752,575 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="es-MX" sz="500" kern="1200"/>
+          <a:endParaRPr lang="es-MX" sz="1200" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7852951" y="1631619"/>
-        <a:ext cx="1146607" cy="56290"/>
+        <a:off x="8835216" y="2671743"/>
+        <a:ext cx="1161586" cy="62649"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{5DC9F435-2CE6-4405-AD55-3577C8FF29E2}">
+  </dsp:spTree>
+</dsp:drawing>
+</file>
+
+<file path=xl/diagrams/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<dsp:drawing xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <dsp:spTree>
+    <dsp:nvGrpSpPr>
+      <dsp:cNvPr id="0" name=""/>
+      <dsp:cNvGrpSpPr/>
+    </dsp:nvGrpSpPr>
+    <dsp:grpSpPr/>
+    <dsp:sp modelId="{21D7A521-1538-481C-B39C-470531060D2B}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6935210" y="2164719"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="8536919" y="1918778"/>
+          <a:ext cx="220455" cy="645967"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="645967"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="220455" y="645967"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{8BD3267A-0DF6-42D0-85DA-6F6A95524E02}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="8316463" y="1918778"/>
+          <a:ext cx="220455" cy="645967"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="220455" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="220455" y="645967"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="645967"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{950FE45F-1099-4E95-8D4E-913F13C39CEE}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="5073791" y="864440"/>
+          <a:ext cx="3463127" cy="386095"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="230172"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="3463127" y="230172"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="3463127" y="386095"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{56AF3754-D66D-47CF-BB3D-6405D6803EB4}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="5068294" y="1918778"/>
+          <a:ext cx="225953" cy="645967"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="645967"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="225953" y="645967"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{A31AE374-C75B-4F82-85A0-BA801DA6BA15}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4853336" y="1918778"/>
+          <a:ext cx="214958" cy="645967"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="214958" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="214958" y="645967"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="645967"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{76481423-7BFC-4E53-B671-E3176BEF8A58}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="5022574" y="864440"/>
+          <a:ext cx="91440" cy="386095"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="51217" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="51217" y="230172"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="45720" y="230172"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="45720" y="386095"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{3C06400A-D79E-462D-AFF3-5E0D57D80F42}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1610664" y="1918778"/>
+          <a:ext cx="220455" cy="645967"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="645967"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="220455" y="645967"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{89DAD94D-D421-4351-AF61-14E572D4FBB0}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1390208" y="1918778"/>
+          <a:ext cx="220455" cy="645967"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="220455" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="220455" y="645967"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="645967"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{F73247A5-92F9-45B3-A4B2-CB760233752E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1610664" y="864440"/>
+          <a:ext cx="3463127" cy="386095"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="3463127" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="3463127" y="230172"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="230172"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="386095"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{3F666415-D5BF-475B-8AAE-39A5A6BA25E5}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4428465" y="196197"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5426,12 +6362,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5444,25 +6380,25 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>Sr. Helios Serrato Pérez</a:t>
+            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
+            <a:t>Consejo de Vigilancia </a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6935210" y="2164719"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="4428465" y="196197"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{8177B874-6A91-4226-9047-656094C7FCA8}">
+    <dsp:sp modelId="{5F1A3974-34FA-4443-A94B-5F13166B2718}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7190012" y="2677761"/>
-          <a:ext cx="1146607" cy="219875"/>
+          <a:off x="4686596" y="715941"/>
+          <a:ext cx="1161586" cy="222747"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5522,24 +6458,24 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>Propietario</a:t>
+            <a:t>2022-2025</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7190012" y="2677761"/>
-        <a:ext cx="1146607" cy="219875"/>
+        <a:off x="4686596" y="715941"/>
+        <a:ext cx="1161586" cy="222747"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{37FA40A9-D75C-44AF-B413-F0C3A4F49306}">
+    <dsp:sp modelId="{9ED8802D-6851-4628-9575-5CD454ED0A4D}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8644445" y="2164719"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="965338" y="1250535"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5581,12 +6517,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5599,25 +6535,25 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>Ing. Noel Javier Ramírez Mejía</a:t>
+            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
+            <a:t>Presidente</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="8644445" y="2164719"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="965338" y="1250535"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{2A16CEDE-4BA4-49BA-AE16-DDE0D3D966CA}">
+    <dsp:sp modelId="{F72357A0-A2DF-42C9-9A9D-2F404917D7F8}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8899246" y="2677761"/>
-          <a:ext cx="1146607" cy="219875"/>
+          <a:off x="1061868" y="1688666"/>
+          <a:ext cx="1161586" cy="57025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5658,12 +6594,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="30480" tIns="7620" rIns="30480" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5675,578 +6611,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>Suplente</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="8899246" y="2677761"/>
-        <a:ext cx="1146607" cy="219875"/>
+        <a:off x="1061868" y="1688666"/>
+        <a:ext cx="1161586" cy="57025"/>
       </dsp:txXfrm>
     </dsp:sp>
-  </dsp:spTree>
-</dsp:drawing>
-</file>
-
-<file path=xl/diagrams/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<dsp:drawing xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <dsp:spTree>
-    <dsp:nvGrpSpPr>
-      <dsp:cNvPr id="0" name=""/>
-      <dsp:cNvGrpSpPr/>
-    </dsp:nvGrpSpPr>
-    <dsp:grpSpPr/>
-    <dsp:sp modelId="{21D7A521-1538-481C-B39C-470531060D2B}">
+    <dsp:sp modelId="{13E60599-934D-435E-972C-34B728BDD199}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8426832" y="1877345"/>
-          <a:ext cx="217612" cy="637637"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="0" y="637637"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="217612" y="637637"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{8BD3267A-0DF6-42D0-85DA-6F6A95524E02}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="8209219" y="1877345"/>
-          <a:ext cx="217612" cy="637637"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="217612" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="217612" y="637637"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="637637"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{950FE45F-1099-4E95-8D4E-913F13C39CEE}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5008363" y="836603"/>
-          <a:ext cx="3418469" cy="381116"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="0" y="227204"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="3418469" y="227204"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="3418469" y="381116"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{56AF3754-D66D-47CF-BB3D-6405D6803EB4}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5002936" y="1877345"/>
-          <a:ext cx="223039" cy="637637"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="0" y="637637"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="223039" y="637637"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{A31AE374-C75B-4F82-85A0-BA801DA6BA15}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4790750" y="1877345"/>
-          <a:ext cx="212186" cy="637637"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="212186" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="212186" y="637637"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="637637"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{76481423-7BFC-4E53-B671-E3176BEF8A58}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4957216" y="836603"/>
-          <a:ext cx="91440" cy="381116"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="51146" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="51146" y="227204"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="45720" y="227204"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="45720" y="381116"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{3C06400A-D79E-462D-AFF3-5E0D57D80F42}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="1589893" y="1877345"/>
-          <a:ext cx="217612" cy="637637"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="0" y="637637"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="217612" y="637637"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{89DAD94D-D421-4351-AF61-14E572D4FBB0}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="1372280" y="1877345"/>
-          <a:ext cx="217612" cy="637637"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="217612" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="217612" y="637637"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="637637"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{F73247A5-92F9-45B3-A4B2-CB760233752E}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="1589893" y="836603"/>
-          <a:ext cx="3418469" cy="381116"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="3418469" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="3418469" y="227204"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="227204"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="381116"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{3F666415-D5BF-475B-8AAE-39A5A6BA25E5}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4371358" y="176977"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="99556" y="2230624"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6288,7 +6669,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -6307,24 +6688,24 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Consejo de Vigilancia </a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4371358" y="176977"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="99556" y="2230624"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{5F1A3974-34FA-4443-A94B-5F13166B2718}">
+    <dsp:sp modelId="{BA5351DA-6F80-47C8-BBCF-ADA0411DC43C}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4626160" y="690019"/>
-          <a:ext cx="1146607" cy="219875"/>
+          <a:off x="150622" y="2716504"/>
+          <a:ext cx="1161586" cy="58560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6365,12 +6746,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="30480" tIns="7620" rIns="30480" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="27940" tIns="6985" rIns="27940" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6382,26 +6763,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>2022-2025</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1100" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4626160" y="690019"/>
-        <a:ext cx="1146607" cy="219875"/>
+        <a:off x="150622" y="2716504"/>
+        <a:ext cx="1161586" cy="58560"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{9ED8802D-6851-4628-9575-5CD454ED0A4D}">
+    <dsp:sp modelId="{3247D56F-F64A-4433-88EA-A164DC2F9628}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="952889" y="1217719"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="1831120" y="2230624"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6443,7 +6821,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -6462,24 +6840,24 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Presidente</a:t>
+            <a:t>Suplente</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="952889" y="1217719"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="1831120" y="2230624"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{F72357A0-A2DF-42C9-9A9D-2F404917D7F8}">
+    <dsp:sp modelId="{1DD63F7F-9D5F-401A-963D-31060E539491}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1048175" y="1650200"/>
-          <a:ext cx="1146607" cy="56290"/>
+          <a:off x="1898750" y="2708224"/>
+          <a:ext cx="1161586" cy="58558"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6520,12 +6898,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="27940" tIns="6985" rIns="27940" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6537,23 +6915,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="es-MX" sz="500" kern="1200"/>
+          <a:endParaRPr lang="es-MX" sz="1100" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1048175" y="1650200"/>
-        <a:ext cx="1146607" cy="56290"/>
+        <a:off x="1898750" y="2708224"/>
+        <a:ext cx="1161586" cy="58558"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{13E60599-934D-435E-972C-34B728BDD199}">
+    <dsp:sp modelId="{5DD61981-23C1-45CB-816C-E7FC3C54CBAE}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="98272" y="2185170"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="4422968" y="1250535"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6595,7 +6973,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -6614,24 +6992,24 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Lic. Gustavo Rodríguez Cabrales</a:t>
+            <a:t>Secretario</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="98272" y="2185170"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="4422968" y="1250535"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{BA5351DA-6F80-47C8-BBCF-ADA0411DC43C}">
+    <dsp:sp modelId="{DAFF9247-F0DB-441E-8679-2A16A7188832}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm>
-          <a:off x="353074" y="2698212"/>
-          <a:ext cx="1146607" cy="219875"/>
+        <a:xfrm flipV="1">
+          <a:off x="4475922" y="1678678"/>
+          <a:ext cx="1183575" cy="57025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6672,12 +7050,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="27940" tIns="6985" rIns="27940" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6689,26 +7067,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Propietario</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="353074" y="2698212"/>
-        <a:ext cx="1146607" cy="219875"/>
+      <dsp:txXfrm rot="10800000">
+        <a:off x="4475922" y="1678678"/>
+        <a:ext cx="1183575" cy="57025"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{3247D56F-F64A-4433-88EA-A164DC2F9628}">
+    <dsp:sp modelId="{22BD4AE8-0E96-4AF3-941E-AFBF8514EA1F}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1807506" y="2185170"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="3562683" y="2230624"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6750,7 +7125,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -6769,24 +7144,24 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>LAE. Esteban Abraham Macari</a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1807506" y="2185170"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="3562683" y="2230624"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{1DD63F7F-9D5F-401A-963D-31060E539491}">
+    <dsp:sp modelId="{88CFCF9E-3D38-4F8A-BED2-E36F336DF41F}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2062308" y="2698212"/>
-          <a:ext cx="1146607" cy="219875"/>
+        <a:xfrm flipV="1">
+          <a:off x="3630314" y="2724791"/>
+          <a:ext cx="1161586" cy="58553"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6844,26 +7219,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Suplente</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1100" kern="1200"/>
         </a:p>
       </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2062308" y="2698212"/>
-        <a:ext cx="1146607" cy="219875"/>
+      <dsp:txXfrm rot="10800000">
+        <a:off x="3630314" y="2724791"/>
+        <a:ext cx="1161586" cy="58553"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{5DD61981-23C1-45CB-816C-E7FC3C54CBAE}">
+    <dsp:sp modelId="{99276632-6755-4F04-94C2-7FD5F7A54AE1}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4365932" y="1217719"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="5294247" y="2230624"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6905,12 +7277,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6923,25 +7295,25 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Secretario</a:t>
+            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
+            <a:t>Suplente</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4365932" y="1217719"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="5294247" y="2230624"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{DAFF9247-F0DB-441E-8679-2A16A7188832}">
+    <dsp:sp modelId="{FFF0DEBF-825F-46FE-B32D-91D5510B0FF6}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4418203" y="1640341"/>
-          <a:ext cx="1168313" cy="56290"/>
+        <a:xfrm>
+          <a:off x="5378442" y="2716509"/>
+          <a:ext cx="1161586" cy="58555"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6982,12 +7354,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="30480" tIns="7620" rIns="30480" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6999,23 +7371,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="es-MX" sz="500" kern="1200"/>
+          <a:endParaRPr lang="es-MX" sz="1200" kern="1200"/>
         </a:p>
       </dsp:txBody>
-      <dsp:txXfrm rot="10800000">
-        <a:off x="4418203" y="1640341"/>
-        <a:ext cx="1168313" cy="56290"/>
+      <dsp:txXfrm>
+        <a:off x="5378442" y="2716509"/>
+        <a:ext cx="1161586" cy="58555"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{22BD4AE8-0E96-4AF3-941E-AFBF8514EA1F}">
+    <dsp:sp modelId="{15ECEB10-3A4A-46CF-BC89-CA90D33E60BE}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3516741" y="2185170"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="7891593" y="1250535"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7057,7 +7429,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -7076,24 +7448,24 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>MVZ. Tito Germán de Coss Tovilla</a:t>
+            <a:t>Tesorero</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3516741" y="2185170"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="7891593" y="1250535"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{88CFCF9E-3D38-4F8A-BED2-E36F336DF41F}">
+    <dsp:sp modelId="{DDC5D6E6-CDD3-4B39-A20A-FECE67469267}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3771543" y="2698212"/>
-          <a:ext cx="1146607" cy="219875"/>
+          <a:off x="7955541" y="1690559"/>
+          <a:ext cx="1161586" cy="57025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7134,12 +7506,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="27940" tIns="6985" rIns="27940" bIns="6985" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7151,26 +7523,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Propietario</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3771543" y="2698212"/>
-        <a:ext cx="1146607" cy="219875"/>
+        <a:off x="7955541" y="1690559"/>
+        <a:ext cx="1161586" cy="57025"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{99276632-6755-4F04-94C2-7FD5F7A54AE1}">
+    <dsp:sp modelId="{5DC9F435-2CE6-4405-AD55-3577C8FF29E2}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5225976" y="2185170"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="7025811" y="2230624"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7212,7 +7581,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -7231,24 +7600,24 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>Ing. Jorge Antonio Salazar Barragán</a:t>
+            <a:t>Propietario</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5225976" y="2185170"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="7025811" y="2230624"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{FFF0DEBF-825F-46FE-B32D-91D5510B0FF6}">
+    <dsp:sp modelId="{8177B874-6A91-4226-9047-656094C7FCA8}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5480777" y="2698212"/>
-          <a:ext cx="1146607" cy="219875"/>
+          <a:off x="7093441" y="2708225"/>
+          <a:ext cx="1161586" cy="58555"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7306,26 +7675,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>Suplente</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1200" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5480777" y="2698212"/>
-        <a:ext cx="1146607" cy="219875"/>
+        <a:off x="7093441" y="2708225"/>
+        <a:ext cx="1161586" cy="58555"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{15ECEB10-3A4A-46CF-BC89-CA90D33E60BE}">
+    <dsp:sp modelId="{37FA40A9-D75C-44AF-B413-F0C3A4F49306}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7789827" y="1217719"/>
-          <a:ext cx="1274008" cy="659625"/>
+          <a:off x="8757375" y="2230624"/>
+          <a:ext cx="1290652" cy="668242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7367,12 +7733,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6985" tIns="6985" rIns="6985" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="94296" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="488950">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7385,25 +7751,25 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Tesorero</a:t>
+            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
+            <a:t>Suplente</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7789827" y="1217719"/>
-        <a:ext cx="1274008" cy="659625"/>
+        <a:off x="8757375" y="2230624"/>
+        <a:ext cx="1290652" cy="668242"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{DDC5D6E6-CDD3-4B39-A20A-FECE67469267}">
+    <dsp:sp modelId="{2A16CEDE-4BA4-49BA-AE16-DDE0D3D966CA}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7852951" y="1652069"/>
-          <a:ext cx="1146607" cy="56290"/>
+          <a:off x="8833287" y="2716504"/>
+          <a:ext cx="1161586" cy="58560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7444,158 +7810,6 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="3175" rIns="12700" bIns="3175" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="222250">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:endParaRPr lang="es-MX" sz="500" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="7852951" y="1652069"/>
-        <a:ext cx="1146607" cy="56290"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{5DC9F435-2CE6-4405-AD55-3577C8FF29E2}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="6935210" y="2185170"/>
-          <a:ext cx="1274008" cy="659625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>Ing. Lauro Aniceto Flores Ramos</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="6935210" y="2185170"/>
-        <a:ext cx="1274008" cy="659625"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{8177B874-6A91-4226-9047-656094C7FCA8}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="7190012" y="2698212"/>
-          <a:ext cx="1146607" cy="219875"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="90000"/>
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-      <dsp:txBody>
         <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="30480" tIns="7620" rIns="30480" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
@@ -7613,170 +7827,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>Propietario</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1200" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7190012" y="2698212"/>
-        <a:ext cx="1146607" cy="219875"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{37FA40A9-D75C-44AF-B413-F0C3A4F49306}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="8644445" y="2185170"/>
-          <a:ext cx="1274008" cy="659625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="93080" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>MVZ. Rene Loyo García</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="8644445" y="2185170"/>
-        <a:ext cx="1274008" cy="659625"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{2A16CEDE-4BA4-49BA-AE16-DDE0D3D966CA}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="8899246" y="2698212"/>
-          <a:ext cx="1146607" cy="219875"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="90000"/>
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="30480" tIns="7620" rIns="30480" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1200" kern="1200"/>
-            <a:t>Suplente</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="8899246" y="2698212"/>
-        <a:ext cx="1146607" cy="219875"/>
+        <a:off x="8833287" y="2716504"/>
+        <a:ext cx="1161586" cy="58560"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -12609,8 +12665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC7D659-D9E1-49E5-8FB4-464D942CFC21}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N60" sqref="N60"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12618,7 +12674,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <webPublishItems count="1">
-    <webPublishItem id="26039" divId="Book1_26039" sourceType="sheet" destinationFile="D:\Dropbox (Personal)\Proyectos\demos\orgchart.htm" autoRepublish="1"/>
+    <webPublishItem id="26039" divId="Book1_26039" sourceType="sheet" destinationFile="D:\Dropbox (Personal)\Proyectos\demos\consejos.htm" autoRepublish="1"/>
   </webPublishItems>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v20240705 - Ajustes de las observaciones del documento
</commit_message>
<xml_diff>
--- a/assets/consejos.xlsx
+++ b/assets/consejos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Personal)\Proyectos\FanCampo\dev\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DBFFF9-90C8-411B-826F-1669DB8B5125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2424DF1A-B192-4AB5-A06C-F5B5560C4260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{63C9C974-292F-4EBA-9C08-E5656FFA8A86}"/>
+    <workbookView xWindow="40080" yWindow="-8250" windowWidth="16440" windowHeight="29040" xr2:uid="{63C9C974-292F-4EBA-9C08-E5656FFA8A86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2849,7 +2849,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Tesorero</a:t>
+            <a:t>Vocal</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -7448,7 +7448,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="es-MX" sz="1100" kern="1200"/>
-            <a:t>Tesorero</a:t>
+            <a:t>Vocal</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
@@ -12665,8 +12665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC7D659-D9E1-49E5-8FB4-464D942CFC21}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>